<commit_message>
Add test for count autodetection
</commit_message>
<xml_diff>
--- a/test/tests.xlsx
+++ b/test/tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgracia\Documents\flies_survival\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgracia\Documents\flies_survival\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C8A510-418C-4DD3-A377-FAA6D44F3E5D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6E0280-BA66-4E24-94DE-AFDD9B18DFA1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3675" windowHeight="3195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dead" sheetId="10" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="dead+unaccounted" sheetId="9" r:id="rId3"/>
     <sheet name="dead+escaped+unaccounted" sheetId="13" r:id="rId4"/>
     <sheet name="dead+escaped+unaccounted+final" sheetId="14" r:id="rId5"/>
+    <sheet name="auto_count" sheetId="16" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="8">
   <si>
     <t>tube</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>1+1</t>
+  </si>
+  <si>
+    <t>:3</t>
   </si>
 </sst>
 </file>
@@ -182,7 +186,61 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -631,23 +689,23 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:AG47"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.0625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="33" width="9.125" style="4" customWidth="1"/>
-    <col min="34" max="16384" width="9" style="4"/>
+    <col min="3" max="34" width="9.125" style="4" customWidth="1"/>
+    <col min="35" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -700,8 +758,9 @@
       <c r="AD1" s="14"/>
       <c r="AE1" s="14"/>
       <c r="AF1" s="14"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AG1" s="14"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -754,6 +813,670 @@
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="5"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D11" s="5"/>
+      <c r="AH11" s="5"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D12" s="5"/>
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D13" s="5"/>
+      <c r="AH13" s="5"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D14" s="5"/>
+      <c r="AD14" s="5"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D15" s="5"/>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="17" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E17" s="5"/>
+      <c r="AA17" s="5"/>
+    </row>
+    <row r="18" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E18" s="5"/>
+      <c r="AG18" s="5"/>
+    </row>
+    <row r="19" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E19" s="5"/>
+      <c r="V19" s="5"/>
+    </row>
+    <row r="20" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E20" s="5"/>
+      <c r="AD20" s="5"/>
+    </row>
+    <row r="21" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E21" s="5"/>
+      <c r="AH21" s="5"/>
+    </row>
+    <row r="27" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="33" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="5:9" x14ac:dyDescent="0.45">
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="AJ2:BA2 AJ3:AN3 C7:BA37 C2:F6 K5:BA6 K4:AN4 K2:AI3">
+    <cfRule type="beginsWith" dxfId="20" priority="4" stopIfTrue="1" operator="beginsWith" text=":">
+      <formula>LEFT(C2,LEN(":"))=":"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:J6">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+      <formula>LEFT(G2,LEN(":"))=":"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" stopIfTrue="1" operator="containsText" id="{9609A0D6-D5F6-4B07-B114-14C838AF3531}">
+            <xm:f>NOT(ISERROR(SEARCH("+",C2)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AJ2:BA2 AJ3:AL3 AN3:BA4 C7:BA37 C2:F6 K5:BA6 K2:AI3 K4:AL4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{87CC7CE2-8AE2-4762-84C7-5E326FA5CACC}">
+            <xm:f>NOT(ISERROR(SEARCH("+",G2)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:J6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248FB839-F167-4274-B33C-990F07C111F7}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:AG47"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.0625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="33" width="9.125" style="4" customWidth="1"/>
+    <col min="34" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14">
+        <v>43101</v>
+      </c>
+      <c r="D1" s="14">
+        <v>43102</v>
+      </c>
+      <c r="E1" s="14">
+        <v>43103</v>
+      </c>
+      <c r="F1" s="14">
+        <v>43104</v>
+      </c>
+      <c r="G1" s="14">
+        <v>43105</v>
+      </c>
+      <c r="H1" s="14">
+        <v>43106</v>
+      </c>
+      <c r="I1" s="14">
+        <v>43107</v>
+      </c>
+      <c r="J1" s="14">
+        <v>43108</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
@@ -766,7 +1489,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -774,8 +1497,8 @@
       <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -906,10 +1629,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
@@ -1202,621 +1925,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{9609A0D6-D5F6-4B07-B114-14C838AF3531}">
-            <xm:f>NOT(ISERROR(SEARCH("+",C2)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <font>
-                <color auto="1"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFEB9C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C4:AK4 AI2:AZ2 C2:AH3 AI3:AK3 C5:AZ37 AM3:AZ4</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248FB839-F167-4274-B33C-990F07C111F7}">
-  <sheetPr>
-    <pageSetUpPr autoPageBreaks="0"/>
-  </sheetPr>
-  <dimension ref="A1:AG47"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="68" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="9.0625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="33" width="9.125" style="4" customWidth="1"/>
-    <col min="34" max="16384" width="9" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14">
-        <v>43101</v>
-      </c>
-      <c r="D1" s="14">
-        <v>43102</v>
-      </c>
-      <c r="E1" s="14">
-        <v>43103</v>
-      </c>
-      <c r="F1" s="14">
-        <v>43104</v>
-      </c>
-      <c r="G1" s="14">
-        <v>43105</v>
-      </c>
-      <c r="H1" s="14">
-        <v>43106</v>
-      </c>
-      <c r="I1" s="14">
-        <v>43107</v>
-      </c>
-      <c r="J1" s="14">
-        <v>43108</v>
-      </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="B7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="B8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="B9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="5"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="D11" s="5"/>
-      <c r="AG11" s="5"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="D12" s="5"/>
-      <c r="Z12" s="5"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="D13" s="5"/>
-      <c r="AG13" s="5"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="D14" s="5"/>
-      <c r="AC14" s="5"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="D15" s="5"/>
-      <c r="W15" s="5"/>
-    </row>
-    <row r="17" spans="4:33" x14ac:dyDescent="0.45">
-      <c r="E17" s="5"/>
-      <c r="Z17" s="5"/>
-    </row>
-    <row r="18" spans="4:33" x14ac:dyDescent="0.45">
-      <c r="E18" s="5"/>
-      <c r="AF18" s="5"/>
-    </row>
-    <row r="19" spans="4:33" x14ac:dyDescent="0.45">
-      <c r="E19" s="5"/>
-      <c r="U19" s="5"/>
-    </row>
-    <row r="20" spans="4:33" x14ac:dyDescent="0.45">
-      <c r="E20" s="5"/>
-      <c r="AC20" s="5"/>
-    </row>
-    <row r="21" spans="4:33" x14ac:dyDescent="0.45">
-      <c r="E21" s="5"/>
-      <c r="AG21" s="5"/>
-    </row>
-    <row r="27" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="33" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E37" s="8"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E42" s="8"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E45" s="8"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E46" s="8"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.45">
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
-      <formula>LEFT(C2,LEN(":"))=":"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2422,10 +2534,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:AK4 AI2:AZ2 C2:AH3 C5:AZ37 D3:AM9">
-    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3031,10 +3143,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3076,7 +3188,7 @@
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3206,10 +3318,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -3220,7 +3332,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -3640,10 +3752,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3673,4 +3785,603 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B942B0CE-6459-4657-BD33-4B5FD70E3B44}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:AG47"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.0625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="33" width="9.125" style="4" customWidth="1"/>
+    <col min="34" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14">
+        <v>43101</v>
+      </c>
+      <c r="D1" s="14">
+        <v>43102</v>
+      </c>
+      <c r="E1" s="14">
+        <v>43103</v>
+      </c>
+      <c r="F1" s="14">
+        <v>43104</v>
+      </c>
+      <c r="G1" s="14">
+        <v>43105</v>
+      </c>
+      <c r="H1" s="14">
+        <v>43106</v>
+      </c>
+      <c r="I1" s="14">
+        <v>43107</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="5"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="D11" s="5"/>
+      <c r="AG11" s="5"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="D12" s="5"/>
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="D13" s="5"/>
+      <c r="AG13" s="5"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="D14" s="5"/>
+      <c r="AC14" s="5"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="D15" s="5"/>
+      <c r="W15" s="5"/>
+    </row>
+    <row r="17" spans="4:33" x14ac:dyDescent="0.45">
+      <c r="E17" s="5"/>
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18" spans="4:33" x14ac:dyDescent="0.45">
+      <c r="E18" s="5"/>
+      <c r="AF18" s="5"/>
+    </row>
+    <row r="19" spans="4:33" x14ac:dyDescent="0.45">
+      <c r="E19" s="5"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="4:33" x14ac:dyDescent="0.45">
+      <c r="E20" s="5"/>
+      <c r="AC20" s="5"/>
+    </row>
+    <row r="21" spans="4:33" x14ac:dyDescent="0.45">
+      <c r="E21" s="5"/>
+      <c r="AG21" s="5"/>
+    </row>
+    <row r="27" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="4:33" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="33" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="5:8" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+      <formula>LEFT(C2,LEN(":"))=":"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{1FB8C910-9ADF-42EE-B24A-FD6BE7B40D4D}">
+            <xm:f>NOT(ISERROR(SEARCH("+",C2)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C4:AK4 AI2:AZ2 C2:AH3 AI3:AK3 C5:AZ37 AM3:AZ4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Support dates and hours timeseries
</commit_message>
<xml_diff>
--- a/test/tests.xlsx
+++ b/test/tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgracia\Documents\flies_survival\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6E0280-BA66-4E24-94DE-AFDD9B18DFA1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C0F01F-58F9-458C-A33A-89141FF8EBC6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3675" windowHeight="3195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3675" windowHeight="3195" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dead" sheetId="10" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="dead+escaped+unaccounted" sheetId="13" r:id="rId4"/>
     <sheet name="dead+escaped+unaccounted+final" sheetId="14" r:id="rId5"/>
     <sheet name="auto_count" sheetId="16" r:id="rId6"/>
+    <sheet name="hours" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="16">
   <si>
     <t>tube</t>
   </si>
@@ -54,6 +55,30 @@
   </si>
   <si>
     <t>:3</t>
+  </si>
+  <si>
+    <t>16h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>24h</t>
+  </si>
+  <si>
+    <t>48h</t>
+  </si>
+  <si>
+    <t>100h</t>
+  </si>
+  <si>
+    <t>200h</t>
+  </si>
+  <si>
+    <t>2h</t>
   </si>
 </sst>
 </file>
@@ -186,7 +211,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="27">
     <dxf>
       <font>
         <color auto="1"/>
@@ -194,6 +219,33 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -356,6 +408,33 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -691,7 +770,7 @@
   </sheetPr>
   <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="68" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
@@ -1289,18 +1368,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AJ2:BA2 AJ3:AN3 C7:BA37 C2:F6 K5:BA6 K4:AN4 K2:AI3">
-    <cfRule type="beginsWith" dxfId="20" priority="4" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="26" priority="4" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:J6">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="24" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(G2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1925,10 +2004,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2534,10 +2613,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:AK4 AI2:AZ2 C2:AH3 C5:AZ37 D3:AM9">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3143,10 +3222,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3752,10 +3831,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4351,10 +4430,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AZ2 C2:AH3 C5:AZ37 C4:AM4 AI3:AM3">
-    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
       <formula>LEFT(C2,LEN(":"))=":"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4384,4 +4463,669 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0F83F1-315C-4079-B3E0-902DB684287F}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:AH47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.0625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="34" width="9.125" style="4" customWidth="1"/>
+    <col min="35" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="5"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D11" s="5"/>
+      <c r="AH11" s="5"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D12" s="5"/>
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D13" s="5"/>
+      <c r="AH13" s="5"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D14" s="5"/>
+      <c r="AD14" s="5"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="D15" s="5"/>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="17" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E17" s="5"/>
+      <c r="AA17" s="5"/>
+    </row>
+    <row r="18" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E18" s="5"/>
+      <c r="AG18" s="5"/>
+    </row>
+    <row r="19" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E19" s="5"/>
+      <c r="V19" s="5"/>
+    </row>
+    <row r="20" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E20" s="5"/>
+      <c r="AD20" s="5"/>
+    </row>
+    <row r="21" spans="4:34" x14ac:dyDescent="0.45">
+      <c r="E21" s="5"/>
+      <c r="AH21" s="5"/>
+    </row>
+    <row r="27" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="4:34" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="33" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="5:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="5:9" x14ac:dyDescent="0.45">
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="AJ2:BA2 AJ3:AN3 C7:BA37 C2:F6 K5:BA6 K4:AN4 K2:AI3">
+    <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text=":">
+      <formula>LEFT(C2,LEN(":"))=":"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:J6">
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="beginsWith" text=":">
+      <formula>LEFT(G2,LEN(":"))=":"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" stopIfTrue="1" operator="containsText" id="{C9C4D06B-9216-41E2-9385-E7D58D908A89}">
+            <xm:f>NOT(ISERROR(SEARCH("+",C2)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AJ2:BA2 AJ3:AL3 AN3:BA4 C7:BA37 C2:F6 K5:BA6 K2:AI3 K4:AL4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{BBE39321-3B3C-483D-8C1A-2CFB00FEA595}">
+            <xm:f>NOT(ISERROR(SEARCH("+",G2)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:J6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>